<commit_message>
v2 is final draft
</commit_message>
<xml_diff>
--- a/LRT.xlsx
+++ b/LRT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theagessler/Documents/Spring 2018/EEOB_563/Final_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{43F2A035-0225-ED4D-B5AA-28689FEBD1BE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{386EAA98-CA69-2D45-9169-601815EB2AC9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="16240" windowHeight="16140" firstSheet="1" activeTab="2" xr2:uid="{1EF10CAE-A4C4-9547-9E7C-F3C9DFC4C38D}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="16240" windowHeight="16140" firstSheet="1" activeTab="3" xr2:uid="{1EF10CAE-A4C4-9547-9E7C-F3C9DFC4C38D}"/>
   </bookViews>
   <sheets>
     <sheet name="SF1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="31">
   <si>
     <t>Tree</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>CPI</t>
+  </si>
+  <si>
+    <t>AM_GG</t>
   </si>
 </sst>
 </file>
@@ -1001,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08596213-D479-7E44-9C4E-07E006758E0F}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1144,6 +1147,18 @@
         <v>-4871.6759949999996</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="6">
+        <v>-4871.0361810000004</v>
+      </c>
+      <c r="C14">
+        <f>2*(B14-B2)</f>
+        <v>1.9923359999993409</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1152,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5719B984-F719-CC41-8182-6BC7A8F25F3C}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1294,6 +1309,18 @@
         <v>-3702.5763980000002</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="6">
+        <v>-3697.1109809999998</v>
+      </c>
+      <c r="C14">
+        <f>2*(B14-B2)</f>
+        <v>14.425136000000748</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>